<commit_message>
(#35) Replaced operation cancellation template
</commit_message>
<xml_diff>
--- a/assets/Шаблон_для_заявки_на_отмену_операции.xlsx
+++ b/assets/Шаблон_для_заявки_на_отмену_операции.xlsx
@@ -1,48 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6720"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Дата проведения операции</t>
-  </si>
-  <si>
-    <t>Номер карты (последние 4 цифры)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>№ п/п в дне7</t>
+  </si>
+  <si>
+    <t>№ п/п в дне8</t>
+  </si>
+  <si>
+    <t>Тип операции</t>
+  </si>
+  <si>
+    <t>Дата проведения</t>
+  </si>
+  <si>
+    <t>Номер пластиковой карты</t>
+  </si>
+  <si>
+    <t>Сумма операции</t>
   </si>
   <si>
     <t>Сумма к отмене</t>
   </si>
   <si>
-    <t>Номер электр. терминала</t>
+    <t>Номер терминала</t>
   </si>
   <si>
     <t>Код авторизации</t>
   </si>
   <si>
-    <t>Примечание</t>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Мерчант</t>
+  </si>
+  <si>
+    <t>Заявка на отмену операций № ____</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -50,7 +88,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -58,15 +134,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -75,53 +157,66 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -130,32 +225,445 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица13" displayName="Таблица13" ref="A2:K4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
+  <tableColumns count="11">
+    <tableColumn id="1" name="№" dataDxfId="10"/>
+    <tableColumn id="7" name="№ п/п в дне7" dataDxfId="9"/>
+    <tableColumn id="8" name="№ п/п в дне8" dataDxfId="8"/>
+    <tableColumn id="9" name="Тип операции" dataDxfId="7"/>
+    <tableColumn id="10" name="Дата проведения" dataDxfId="6"/>
+    <tableColumn id="11" name="Номер пластиковой карты" dataDxfId="5"/>
+    <tableColumn id="12" name="Сумма операции" dataDxfId="4"/>
+    <tableColumn id="13" name="Сумма к отмене" dataDxfId="3"/>
+    <tableColumn id="14" name="Номер терминала" dataDxfId="2"/>
+    <tableColumn id="19" name="Мерчант" dataDxfId="1"/>
+    <tableColumn id="15" name="Код авторизации" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -445,95 +953,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:H10"/>
+  <sheetPr codeName="Лист1"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="0.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="6" customWidth="1"/>
+    <col min="9" max="10" width="16.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="3:8" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="H2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="8" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
     </row>
-    <row r="9" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>